<commit_message>
Feasibility of U2G2 with new screen layout added
</commit_message>
<xml_diff>
--- a/01 System/Projectplan.xlsx
+++ b/01 System/Projectplan.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hj.vanderpol\Documents\IOT\BedClock\01 System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1A391E09-5154-41EA-A989-6F8A08E05B67}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB20B94-4402-421A-8211-7CC6D64A975D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>To do Nightlight</t>
   </si>
@@ -114,12 +114,6 @@
     <t>Find way to record power on event</t>
   </si>
   <si>
-    <t>min scale</t>
-  </si>
-  <si>
-    <t>max scale</t>
-  </si>
-  <si>
     <t>V3.0</t>
   </si>
   <si>
@@ -133,13 +127,16 @@
   </si>
   <si>
     <t>Store project on Github</t>
+  </si>
+  <si>
+    <t>Switch off WiFi if not needed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="15" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,6 +215,17 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Heebo"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Heebo"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Heebo"/>
     </font>
@@ -352,7 +360,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -368,26 +376,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="18">
-    <cellStyle name="Accent" xfId="7"/>
-    <cellStyle name="Accent 1" xfId="8"/>
-    <cellStyle name="Accent 2" xfId="9"/>
-    <cellStyle name="Accent 3" xfId="10"/>
+    <cellStyle name="Accent" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Accent 1" xfId="8" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Accent 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Accent 3" xfId="10" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Bad" xfId="4" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Error" xfId="11"/>
-    <cellStyle name="Footnote" xfId="12"/>
+    <cellStyle name="Error" xfId="11" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Footnote" xfId="12" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Good" xfId="3" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading" xfId="13"/>
+    <cellStyle name="Heading" xfId="13" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="14"/>
+    <cellStyle name="Hyperlink" xfId="14" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Neutral" xfId="5" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Note" xfId="6" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Status" xfId="15"/>
-    <cellStyle name="Text" xfId="16"/>
-    <cellStyle name="Warning" xfId="17"/>
+    <cellStyle name="Status" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Text" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Warning" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -698,15 +715,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
+      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="3.4140625" customWidth="1"/>
     <col min="2" max="2" width="54.1640625" bestFit="1" customWidth="1"/>
@@ -714,7 +731,7 @@
     <col min="4" max="5" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -725,30 +742,30 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="1"/>
-      <c r="C2" s="3">
-        <f>SUM(C$3:C$38)/COUNT(C$3:C$38)</f>
-        <v>1</v>
-      </c>
-      <c r="D2" s="3">
-        <f>SUM(D$3:D$38)/COUNT(D$3:D$38)</f>
-        <v>1</v>
-      </c>
-      <c r="E2" s="3">
-        <f>SUM(E$3:E$38)/COUNT(E$3:E$38)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="5"/>
+      <c r="C2" s="7">
+        <f>SUM(C$3:C$10002)/COUNT(C$3:C$10002)</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="7">
+        <f>SUM(D$3:D$10002)/COUNT(D$3:D$10002)</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="7">
+        <f>SUM(E$3:E$10002)/COUNT(E$3:E$10002)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -756,7 +773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -764,7 +781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -772,7 +789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -780,7 +797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -790,7 +807,7 @@
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -800,7 +817,7 @@
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -810,7 +827,7 @@
       </c>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -820,7 +837,7 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -830,7 +847,7 @@
       </c>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" t="s">
         <v>13</v>
       </c>
@@ -840,7 +857,7 @@
       </c>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -848,7 +865,7 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" t="s">
         <v>15</v>
       </c>
@@ -858,7 +875,7 @@
       </c>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" t="s">
         <v>16</v>
       </c>
@@ -868,7 +885,7 @@
       </c>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" t="s">
         <v>17</v>
       </c>
@@ -878,7 +895,7 @@
       </c>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -886,7 +903,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" t="s">
         <v>19</v>
       </c>
@@ -896,7 +913,7 @@
       </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" t="s">
         <v>20</v>
       </c>
@@ -906,10 +923,10 @@
       </c>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -918,10 +935,10 @@
       </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -929,7 +946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" t="s">
         <v>25</v>
       </c>
@@ -937,95 +954,73 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D28" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E30" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E31" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E32" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
         <v>21</v>
       </c>
-      <c r="C34"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-    </row>
-    <row r="35" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B35" t="s">
+      <c r="C36"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B37" t="s">
         <v>22</v>
       </c>
-      <c r="C35"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3">
+      <c r="C37"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3">
         <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="37" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="38" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="39" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B39" t="s">
-        <v>27</v>
-      </c>
-      <c r="C39" s="3">
-        <v>0</v>
-      </c>
-      <c r="D39" s="3">
-        <v>0</v>
-      </c>
-      <c r="E39" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B40" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40" s="3">
-        <v>1</v>
-      </c>
-      <c r="D40" s="3">
-        <v>1</v>
-      </c>
-      <c r="E40" s="3">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Screen contrast added, including auto screen contrast
</commit_message>
<xml_diff>
--- a/01 System/Projectplan.xlsx
+++ b/01 System/Projectplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hj.vanderpol\Documents\IOT\BedClock\01 System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F713329-BB43-41E9-8AE3-D70D1042BA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56FE225-06ED-4E9B-8850-955364C2AF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>To do Nightlight</t>
   </si>
@@ -166,6 +166,15 @@
   </si>
   <si>
     <t>Monitor status through Telegram</t>
+  </si>
+  <si>
+    <t>Allow user to configure screen contrast</t>
+  </si>
+  <si>
+    <t>Make screen contrast dependent of sunrise and sunset</t>
+  </si>
+  <si>
+    <t>Startup screen</t>
   </si>
 </sst>
 </file>
@@ -762,23 +771,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="3.4140625" customWidth="1"/>
-    <col min="2" max="2" width="54.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" style="7" customWidth="1"/>
-    <col min="4" max="6" width="10.6640625" style="7" customWidth="1"/>
-    <col min="7" max="16384" width="8.6640625" style="7"/>
+    <col min="1" max="1" width="3.3984375" customWidth="1"/>
+    <col min="2" max="2" width="54.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.296875" style="7" customWidth="1"/>
+    <col min="4" max="6" width="10.69921875" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="8.69921875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -795,32 +804,32 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" s="6" customFormat="1" ht="16.2" x14ac:dyDescent="0.5">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="6">
-        <f>SUM(C$3:C$10001)/COUNT(C$3:C$10001)</f>
+        <f>SUM(C$3:C$10004)/COUNT(C$3:C$10004)</f>
         <v>1</v>
       </c>
       <c r="D2" s="6">
-        <f>SUM(D$3:D$10001)/COUNT(D$3:D$10001)</f>
+        <f>SUM(D$3:D$10004)/COUNT(D$3:D$10004)</f>
         <v>1</v>
       </c>
       <c r="E2" s="6">
-        <f>SUM(E$3:E$10001)/COUNT(E$3:E$10001)</f>
+        <f>SUM(E$3:E$10004)/COUNT(E$3:E$10004)</f>
         <v>1</v>
       </c>
       <c r="F2" s="6">
-        <f>SUM(F$3:F$10001)/COUNT(F$3:F$10001)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <f>SUM(F$3:F$10004)/COUNT(F$3:F$10004)</f>
+        <v>3.8461538461538464E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -828,7 +837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -836,7 +845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -844,7 +853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -852,7 +861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -860,7 +869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -868,7 +877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -876,7 +885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -884,7 +893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -892,7 +901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B13" t="s">
         <v>13</v>
       </c>
@@ -900,12 +909,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B15" t="s">
         <v>15</v>
       </c>
@@ -913,7 +922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B16" t="s">
         <v>16</v>
       </c>
@@ -921,7 +930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B17" t="s">
         <v>17</v>
       </c>
@@ -929,12 +938,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B19" t="s">
         <v>19</v>
       </c>
@@ -942,7 +951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B20" t="s">
         <v>20</v>
       </c>
@@ -950,7 +959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -958,7 +967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A24" s="5" t="s">
         <v>23</v>
       </c>
@@ -967,7 +976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A25" s="5"/>
       <c r="B25" s="5" t="s">
         <v>24</v>
@@ -976,17 +985,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A26" s="5"/>
       <c r="B26" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -994,7 +1003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -1002,7 +1011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B31" t="s">
         <v>28</v>
       </c>
@@ -1010,7 +1019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B32" t="s">
         <v>29</v>
       </c>
@@ -1018,7 +1027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B33" t="s">
         <v>33</v>
       </c>
@@ -1026,12 +1035,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B36" t="s">
         <v>31</v>
       </c>
@@ -1039,7 +1048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -1047,85 +1056,109 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B41" t="s">
+        <v>45</v>
+      </c>
+      <c r="F41" s="7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="B42" t="s">
+        <v>46</v>
+      </c>
+      <c r="F42" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="B43" t="s">
+        <v>47</v>
+      </c>
+      <c r="F43" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="B44" t="s">
         <v>35</v>
       </c>
-      <c r="F41" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F42" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B43" t="s">
+      <c r="F44" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="F45" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="B46" t="s">
         <v>38</v>
       </c>
-      <c r="F43" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B44" t="s">
+      <c r="F46" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="B47" t="s">
         <v>39</v>
       </c>
-      <c r="F44" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B45" t="s">
+      <c r="F47" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="B48" t="s">
         <v>40</v>
       </c>
-      <c r="F45" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B46" t="s">
+      <c r="F48" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.5">
+      <c r="B49" t="s">
         <v>37</v>
       </c>
-      <c r="F46" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B48" t="s">
+      <c r="F49" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.5">
+      <c r="B51" t="s">
         <v>41</v>
       </c>
-      <c r="F48" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B50" t="s">
+      <c r="F51" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.5">
+      <c r="B53" t="s">
         <v>42</v>
       </c>
-      <c r="F50" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B52" t="s">
+      <c r="F53" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.5">
+      <c r="B55" t="s">
         <v>43</v>
       </c>
-      <c r="F52" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B54" t="s">
+      <c r="F55" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.5">
+      <c r="B57" t="s">
         <v>44</v>
       </c>
-      <c r="F54" s="7">
+      <c r="F57" s="7">
         <v>0</v>
       </c>
     </row>

</xml_diff>